<commit_message>
Updated JPN model - 2025-08-05 12:04
</commit_message>
<xml_diff>
--- a/VerveStacks_JPN/vt_vervestacks_JPN_v1.xlsx
+++ b/VerveStacks_JPN/vt_vervestacks_JPN_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_JPN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99B8F5D9-C8A1-4374-A440-B59FA66E8528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32F00711-4012-444F-A00D-5B3FFE07DF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{CB8303B4-3443-4077-A1F5-821F4574737B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{2236884D-2E9B-4C69-B78E-13C766611BCE}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -6111,7 +6111,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9F3BA1-122A-4C8A-8C42-7F5032590955}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFFA7F7-D413-4FE9-AA6E-8CC9B77FA2FF}">
   <dimension ref="A2:P102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -8903,7 +8903,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DFB85B-9560-4F06-A912-9E2BCA5686CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2669B265-D55C-4E88-8D6F-7B3C9EC85578}">
   <dimension ref="A2:T394"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -30876,7 +30876,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BA190E-4B9D-48AB-ABC6-E2F7F05FEE3D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB336D3-1759-4BE9-8956-939B8D708F41}">
   <dimension ref="A2:S686"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>